<commit_message>
nC_Dinesh[Fix]-To Cater, Balance Sheet Click Intercept in Firefox
</commit_message>
<xml_diff>
--- a/TestExcels/Elements/nC_Elements.xlsx
+++ b/TestExcels/Elements/nC_Elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium\1. nC\nC_Selenium\TestExcels\Elements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660682BB-6B1A-41A7-9FA7-6AC0D571C5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0B93A2-F5A3-418A-B447-952C9927A7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="4" xr2:uid="{8BE0CCB9-D430-49D3-A8C9-61B6CECA8B37}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{8BE0CCB9-D430-49D3-A8C9-61B6CECA8B37}"/>
   </bookViews>
   <sheets>
     <sheet name="ImportantNotes" sheetId="5" r:id="rId1"/>
@@ -333,7 +333,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="324">
   <si>
     <t>KEY</t>
   </si>
@@ -1498,6 +1498,15 @@
   </si>
   <si>
     <t>XPATH SYNTAX</t>
+  </si>
+  <si>
+    <t>//*[@id='simple-menu']</t>
+  </si>
+  <si>
+    <t>BalSheetClickBlocker</t>
+  </si>
+  <si>
+    <t>This is Blocking the Balance Sheet Click in LMM</t>
   </si>
 </sst>
 </file>
@@ -2716,10 +2725,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2BC4CAE-8D6E-4DF3-A41A-29292F67A959}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2923,6 +2932,17 @@
         <v>196</v>
       </c>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B25" t="s">
+        <v>321</v>
+      </c>
+      <c r="C25" t="s">
+        <v>323</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2934,8 +2954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61D3C10-FD12-45E2-88F4-FE21AA9F5374}">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>